<commit_message>
It takes the number of rows from the training cases dinamically
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t>Genero</t>
   </si>
@@ -397,13 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -485,6 +488,226 @@
         <v>110000</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>70000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Parameters are entered by the user
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Genero</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Hombre</t>
   </si>
   <si>
-    <t>Catamarca</t>
-  </si>
-  <si>
     <t>Universitario</t>
   </si>
   <si>
@@ -47,15 +44,6 @@
   </si>
   <si>
     <t>CABA</t>
-  </si>
-  <si>
-    <t>Posgrado</t>
-  </si>
-  <si>
-    <t>Otros</t>
-  </si>
-  <si>
-    <t>GBA</t>
   </si>
 </sst>
 </file>
@@ -397,15 +385,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -433,59 +423,59 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>80000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>120000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>110000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -493,219 +483,99 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5">
-        <v>50000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>60000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>70000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>70000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10">
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11">
-        <v>110000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>70000</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>